<commit_message>
made changes to models in administration
</commit_message>
<xml_diff>
--- a/sample_data/user.xlsx
+++ b/sample_data/user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\compsci\Semester 4\Python\project2\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2031667\Desktop\project2\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46363CEC-086E-400C-B7F0-9AE3DFD64483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BF80F3-711B-4D67-ACB2-FF820B65105F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>!password7</t>
+  </si>
+  <si>
+    <t>peter.griffin@gmail.com</t>
+  </si>
+  <si>
+    <t>ron.swanson@gmail.com</t>
+  </si>
+  <si>
+    <t>matt.murdock@gmail.com</t>
+  </si>
+  <si>
+    <t>davey.jones@gmail.com</t>
+  </si>
+  <si>
+    <t>nick.cage@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +495,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,7 +523,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,7 +537,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -536,7 +551,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -545,6 +560,11 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{882E36FA-5005-479D-A0F6-6E181E191923}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{64C95A02-2BDD-4D68-80A1-8B663161BBE0}"/>
     <hyperlink ref="D4:D8" r:id="rId3" display="barry.benson@gmail.com" xr:uid="{53CE1EBF-ABB3-4BB2-86A5-E04E3BD6D4EC}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{A0FB5203-A5BA-44E6-B4D3-F783EDEEBF8A}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{4E6B57F6-9744-4A2A-A58D-D1F08998D270}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{14D56DC0-55CD-4BD5-A47F-12D224B757A8}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{5ADC06C8-1C46-4227-BD98-CDBAF879827C}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{4F3C0B3E-3D0C-4108-8618-3321C1792469}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>